<commit_message>
Actualización de la planificación
</commit_message>
<xml_diff>
--- a/Planificación.xlsx
+++ b/Planificación.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tomiabarca/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tomiabarca/Documents/1_Cuatrimestre/ISO2/Practicas/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C95605BA-F467-8A4F-BD10-2EAA49065DE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35B1EF7F-9817-7E4B-87C4-8F6FC4C9C659}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15720" xr2:uid="{1E22A818-5115-4EEC-BACB-97BF20EAB24C}"/>
   </bookViews>
@@ -1065,10 +1065,50 @@
     <xf numFmtId="0" fontId="2" fillId="25" borderId="15" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="27" xfId="12" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="8" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" xfId="10" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1083,12 +1123,6 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="28" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" xfId="10" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="17" borderId="30" xfId="12" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1098,40 +1132,6 @@
     <xf numFmtId="0" fontId="7" fillId="17" borderId="32" xfId="12" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="27" xfId="12" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="6" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="8" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="20% - Énfasis1" xfId="2" builtinId="30"/>
@@ -3260,8 +3260,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCABCBAC-E3CF-4453-A312-13BD53787315}">
   <dimension ref="B1:AI109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A75" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
+    <sheetView tabSelected="1" topLeftCell="A78" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F104" sqref="F104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3743,83 +3743,83 @@
       </c>
     </row>
     <row r="13" spans="2:32" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="93" t="s">
+      <c r="B13" s="97" t="s">
         <v>81</v>
       </c>
-      <c r="C13" s="93"/>
-      <c r="D13" s="93"/>
-      <c r="E13" s="93"/>
-      <c r="F13" s="93"/>
-      <c r="G13" s="93"/>
-      <c r="H13" s="93"/>
-      <c r="I13" s="93"/>
-      <c r="J13" s="93"/>
-      <c r="K13" s="93"/>
-      <c r="L13" s="93"/>
-      <c r="M13" s="93"/>
-      <c r="N13" s="93"/>
-      <c r="O13" s="93"/>
-      <c r="P13" s="93"/>
-      <c r="Q13" s="93"/>
-      <c r="R13" s="93"/>
-      <c r="S13" s="93"/>
-      <c r="T13" s="93"/>
-      <c r="U13" s="93"/>
-      <c r="V13" s="93"/>
-      <c r="W13" s="93"/>
-      <c r="X13" s="93"/>
-      <c r="Y13" s="93"/>
-      <c r="Z13" s="93"/>
-      <c r="AA13" s="93"/>
-      <c r="AB13" s="93"/>
-      <c r="AC13" s="93"/>
-      <c r="AD13" s="93"/>
-      <c r="AE13" s="93"/>
-      <c r="AF13" s="93"/>
+      <c r="C13" s="97"/>
+      <c r="D13" s="97"/>
+      <c r="E13" s="97"/>
+      <c r="F13" s="97"/>
+      <c r="G13" s="97"/>
+      <c r="H13" s="97"/>
+      <c r="I13" s="97"/>
+      <c r="J13" s="97"/>
+      <c r="K13" s="97"/>
+      <c r="L13" s="97"/>
+      <c r="M13" s="97"/>
+      <c r="N13" s="97"/>
+      <c r="O13" s="97"/>
+      <c r="P13" s="97"/>
+      <c r="Q13" s="97"/>
+      <c r="R13" s="97"/>
+      <c r="S13" s="97"/>
+      <c r="T13" s="97"/>
+      <c r="U13" s="97"/>
+      <c r="V13" s="97"/>
+      <c r="W13" s="97"/>
+      <c r="X13" s="97"/>
+      <c r="Y13" s="97"/>
+      <c r="Z13" s="97"/>
+      <c r="AA13" s="97"/>
+      <c r="AB13" s="97"/>
+      <c r="AC13" s="97"/>
+      <c r="AD13" s="97"/>
+      <c r="AE13" s="97"/>
+      <c r="AF13" s="97"/>
     </row>
     <row r="14" spans="2:32" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C14" s="110" t="s">
+      <c r="C14" s="100" t="s">
         <v>0</v>
       </c>
-      <c r="D14" s="110"/>
-      <c r="E14" s="110"/>
-      <c r="F14" s="110"/>
-      <c r="G14" s="110"/>
-      <c r="H14" s="111" t="s">
+      <c r="D14" s="100"/>
+      <c r="E14" s="100"/>
+      <c r="F14" s="100"/>
+      <c r="G14" s="100"/>
+      <c r="H14" s="101" t="s">
         <v>1</v>
       </c>
-      <c r="I14" s="111"/>
-      <c r="J14" s="111"/>
-      <c r="K14" s="111"/>
-      <c r="L14" s="111"/>
-      <c r="M14" s="112" t="s">
+      <c r="I14" s="101"/>
+      <c r="J14" s="101"/>
+      <c r="K14" s="101"/>
+      <c r="L14" s="101"/>
+      <c r="M14" s="102" t="s">
         <v>2</v>
       </c>
-      <c r="N14" s="112"/>
-      <c r="O14" s="112"/>
-      <c r="P14" s="112"/>
-      <c r="Q14" s="112"/>
-      <c r="R14" s="98" t="s">
+      <c r="N14" s="102"/>
+      <c r="O14" s="102"/>
+      <c r="P14" s="102"/>
+      <c r="Q14" s="102"/>
+      <c r="R14" s="103" t="s">
         <v>3</v>
       </c>
-      <c r="S14" s="98"/>
-      <c r="T14" s="98"/>
-      <c r="U14" s="98"/>
-      <c r="V14" s="98"/>
-      <c r="W14" s="99" t="s">
+      <c r="S14" s="103"/>
+      <c r="T14" s="103"/>
+      <c r="U14" s="103"/>
+      <c r="V14" s="103"/>
+      <c r="W14" s="104" t="s">
         <v>4</v>
       </c>
-      <c r="X14" s="99"/>
-      <c r="Y14" s="99"/>
-      <c r="Z14" s="99"/>
-      <c r="AA14" s="99"/>
-      <c r="AB14" s="109" t="s">
+      <c r="X14" s="104"/>
+      <c r="Y14" s="104"/>
+      <c r="Z14" s="104"/>
+      <c r="AA14" s="104"/>
+      <c r="AB14" s="99" t="s">
         <v>5</v>
       </c>
-      <c r="AC14" s="109"/>
-      <c r="AD14" s="109"/>
-      <c r="AE14" s="109"/>
-      <c r="AF14" s="109"/>
+      <c r="AC14" s="99"/>
+      <c r="AD14" s="99"/>
+      <c r="AE14" s="99"/>
+      <c r="AF14" s="99"/>
     </row>
     <row r="15" spans="2:32" ht="16" thickTop="1" x14ac:dyDescent="0.2">
       <c r="B15" s="2" t="s">
@@ -4304,11 +4304,11 @@
       <c r="AF22" s="21">
         <v>1</v>
       </c>
-      <c r="AG22" s="92" t="s">
+      <c r="AG22" s="93" t="s">
         <v>88</v>
       </c>
-      <c r="AH22" s="92"/>
-      <c r="AI22" s="92"/>
+      <c r="AH22" s="93"/>
+      <c r="AI22" s="93"/>
     </row>
     <row r="23" spans="2:35" x14ac:dyDescent="0.2">
       <c r="B23" s="5" t="s">
@@ -4345,28 +4345,28 @@
       <c r="T23" s="64"/>
       <c r="U23" s="64"/>
       <c r="V23" s="65"/>
-      <c r="W23" s="103">
+      <c r="W23" s="94">
         <f>SUM(W17,X17,Y18,Y19,Z20,Z21,AA22)</f>
         <v>18</v>
       </c>
-      <c r="X23" s="104"/>
-      <c r="Y23" s="104"/>
-      <c r="Z23" s="104"/>
-      <c r="AA23" s="105"/>
-      <c r="AB23" s="103">
+      <c r="X23" s="95"/>
+      <c r="Y23" s="95"/>
+      <c r="Z23" s="95"/>
+      <c r="AA23" s="96"/>
+      <c r="AB23" s="94">
         <f>SUM(AB17,AC17,AD18,AD19,AE20,AE21,AF22)</f>
         <v>12</v>
       </c>
-      <c r="AC23" s="104"/>
-      <c r="AD23" s="104"/>
-      <c r="AE23" s="104"/>
-      <c r="AF23" s="105"/>
-      <c r="AG23" s="103">
+      <c r="AC23" s="95"/>
+      <c r="AD23" s="95"/>
+      <c r="AE23" s="95"/>
+      <c r="AF23" s="96"/>
+      <c r="AG23" s="94">
         <f>SUM(AB23,W23,R23,M23,H23,C23)</f>
         <v>153</v>
       </c>
-      <c r="AH23" s="104"/>
-      <c r="AI23" s="105"/>
+      <c r="AH23" s="95"/>
+      <c r="AI23" s="96"/>
     </row>
     <row r="24" spans="2:35" x14ac:dyDescent="0.2">
       <c r="B24" s="5" t="s">
@@ -4400,25 +4400,25 @@
       <c r="T24" s="64"/>
       <c r="U24" s="64"/>
       <c r="V24" s="65"/>
-      <c r="W24" s="103">
+      <c r="W24" s="94">
         <v>540</v>
       </c>
-      <c r="X24" s="104"/>
-      <c r="Y24" s="104"/>
-      <c r="Z24" s="104"/>
-      <c r="AA24" s="105"/>
-      <c r="AB24" s="103">
+      <c r="X24" s="95"/>
+      <c r="Y24" s="95"/>
+      <c r="Z24" s="95"/>
+      <c r="AA24" s="96"/>
+      <c r="AB24" s="94">
         <v>360</v>
       </c>
-      <c r="AC24" s="104"/>
-      <c r="AD24" s="104"/>
-      <c r="AE24" s="104"/>
-      <c r="AF24" s="105"/>
-      <c r="AG24" s="103">
+      <c r="AC24" s="95"/>
+      <c r="AD24" s="95"/>
+      <c r="AE24" s="95"/>
+      <c r="AF24" s="96"/>
+      <c r="AG24" s="94">
         <v>4590</v>
       </c>
-      <c r="AH24" s="104"/>
-      <c r="AI24" s="105"/>
+      <c r="AH24" s="95"/>
+      <c r="AI24" s="96"/>
     </row>
     <row r="25" spans="2:35" x14ac:dyDescent="0.2">
       <c r="B25" s="5" t="s">
@@ -4452,68 +4452,68 @@
       <c r="T25" s="64"/>
       <c r="U25" s="64"/>
       <c r="V25" s="65"/>
-      <c r="W25" s="103">
+      <c r="W25" s="94">
         <v>3</v>
       </c>
-      <c r="X25" s="104"/>
-      <c r="Y25" s="104"/>
-      <c r="Z25" s="104"/>
-      <c r="AA25" s="105"/>
-      <c r="AB25" s="103">
+      <c r="X25" s="95"/>
+      <c r="Y25" s="95"/>
+      <c r="Z25" s="95"/>
+      <c r="AA25" s="96"/>
+      <c r="AB25" s="94">
         <v>2</v>
       </c>
-      <c r="AC25" s="104"/>
-      <c r="AD25" s="104"/>
-      <c r="AE25" s="104"/>
-      <c r="AF25" s="105"/>
-      <c r="AG25" s="103">
+      <c r="AC25" s="95"/>
+      <c r="AD25" s="95"/>
+      <c r="AE25" s="95"/>
+      <c r="AF25" s="96"/>
+      <c r="AG25" s="94">
         <f>SUM(AB25,W25,R25,M25,H25,C25)</f>
         <v>19</v>
       </c>
-      <c r="AH25" s="104"/>
-      <c r="AI25" s="105"/>
+      <c r="AH25" s="95"/>
+      <c r="AI25" s="96"/>
     </row>
     <row r="27" spans="2:35" x14ac:dyDescent="0.2">
-      <c r="C27" s="93" t="s">
+      <c r="C27" s="97" t="s">
         <v>78</v>
       </c>
-      <c r="D27" s="93"/>
-      <c r="E27" s="93"/>
-      <c r="F27" s="93"/>
-      <c r="G27" s="93"/>
-      <c r="H27" s="93"/>
-      <c r="I27" s="93"/>
-      <c r="J27" s="93"/>
-      <c r="K27" s="93"/>
-      <c r="L27" s="93"/>
-      <c r="M27" s="93"/>
-      <c r="N27" s="93"/>
-      <c r="O27" s="93"/>
-      <c r="P27" s="93"/>
-      <c r="Q27" s="93"/>
+      <c r="D27" s="97"/>
+      <c r="E27" s="97"/>
+      <c r="F27" s="97"/>
+      <c r="G27" s="97"/>
+      <c r="H27" s="97"/>
+      <c r="I27" s="97"/>
+      <c r="J27" s="97"/>
+      <c r="K27" s="97"/>
+      <c r="L27" s="97"/>
+      <c r="M27" s="97"/>
+      <c r="N27" s="97"/>
+      <c r="O27" s="97"/>
+      <c r="P27" s="97"/>
+      <c r="Q27" s="97"/>
     </row>
     <row r="28" spans="2:35" x14ac:dyDescent="0.2">
-      <c r="C28" s="95" t="s">
+      <c r="C28" s="109" t="s">
         <v>0</v>
       </c>
-      <c r="D28" s="95"/>
-      <c r="E28" s="95"/>
-      <c r="F28" s="95"/>
-      <c r="G28" s="95"/>
-      <c r="H28" s="96" t="s">
+      <c r="D28" s="109"/>
+      <c r="E28" s="109"/>
+      <c r="F28" s="109"/>
+      <c r="G28" s="109"/>
+      <c r="H28" s="110" t="s">
         <v>1</v>
       </c>
-      <c r="I28" s="96"/>
-      <c r="J28" s="96"/>
-      <c r="K28" s="96"/>
-      <c r="L28" s="96"/>
-      <c r="M28" s="97" t="s">
+      <c r="I28" s="110"/>
+      <c r="J28" s="110"/>
+      <c r="K28" s="110"/>
+      <c r="L28" s="110"/>
+      <c r="M28" s="111" t="s">
         <v>2</v>
       </c>
-      <c r="N28" s="97"/>
-      <c r="O28" s="97"/>
-      <c r="P28" s="97"/>
-      <c r="Q28" s="97"/>
+      <c r="N28" s="111"/>
+      <c r="O28" s="111"/>
+      <c r="P28" s="111"/>
+      <c r="Q28" s="111"/>
     </row>
     <row r="29" spans="2:35" x14ac:dyDescent="0.2">
       <c r="B29" s="5" t="s">
@@ -4778,134 +4778,134 @@
       <c r="O36" s="5"/>
       <c r="P36" s="5"/>
       <c r="Q36" s="5"/>
-      <c r="R36" s="92" t="s">
+      <c r="R36" s="93" t="s">
         <v>88</v>
       </c>
-      <c r="S36" s="92"/>
-      <c r="T36" s="92"/>
+      <c r="S36" s="93"/>
+      <c r="T36" s="93"/>
     </row>
     <row r="37" spans="2:27" x14ac:dyDescent="0.2">
       <c r="B37" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="C37" s="92">
+      <c r="C37" s="93">
         <v>41</v>
       </c>
-      <c r="D37" s="92"/>
-      <c r="E37" s="92"/>
-      <c r="F37" s="92"/>
-      <c r="G37" s="92"/>
-      <c r="H37" s="92">
+      <c r="D37" s="93"/>
+      <c r="E37" s="93"/>
+      <c r="F37" s="93"/>
+      <c r="G37" s="93"/>
+      <c r="H37" s="93">
         <v>16</v>
       </c>
-      <c r="I37" s="92"/>
-      <c r="J37" s="92"/>
-      <c r="K37" s="92"/>
-      <c r="L37" s="92"/>
-      <c r="M37" s="92">
+      <c r="I37" s="93"/>
+      <c r="J37" s="93"/>
+      <c r="K37" s="93"/>
+      <c r="L37" s="93"/>
+      <c r="M37" s="93">
         <v>16</v>
       </c>
-      <c r="N37" s="92"/>
-      <c r="O37" s="92"/>
-      <c r="P37" s="92"/>
-      <c r="Q37" s="92"/>
-      <c r="R37" s="103">
+      <c r="N37" s="93"/>
+      <c r="O37" s="93"/>
+      <c r="P37" s="93"/>
+      <c r="Q37" s="93"/>
+      <c r="R37" s="94">
         <v>73</v>
       </c>
-      <c r="S37" s="104"/>
-      <c r="T37" s="105"/>
+      <c r="S37" s="95"/>
+      <c r="T37" s="96"/>
     </row>
     <row r="38" spans="2:27" x14ac:dyDescent="0.2">
       <c r="B38" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="C38" s="92">
+      <c r="C38" s="93">
         <v>1230</v>
       </c>
-      <c r="D38" s="92"/>
-      <c r="E38" s="92"/>
-      <c r="F38" s="92"/>
-      <c r="G38" s="92"/>
-      <c r="H38" s="92">
+      <c r="D38" s="93"/>
+      <c r="E38" s="93"/>
+      <c r="F38" s="93"/>
+      <c r="G38" s="93"/>
+      <c r="H38" s="93">
         <v>480</v>
       </c>
-      <c r="I38" s="92"/>
-      <c r="J38" s="92"/>
-      <c r="K38" s="92"/>
-      <c r="L38" s="92"/>
-      <c r="M38" s="92">
+      <c r="I38" s="93"/>
+      <c r="J38" s="93"/>
+      <c r="K38" s="93"/>
+      <c r="L38" s="93"/>
+      <c r="M38" s="93">
         <v>480</v>
       </c>
-      <c r="N38" s="92"/>
-      <c r="O38" s="92"/>
-      <c r="P38" s="92"/>
-      <c r="Q38" s="92"/>
-      <c r="R38" s="103">
+      <c r="N38" s="93"/>
+      <c r="O38" s="93"/>
+      <c r="P38" s="93"/>
+      <c r="Q38" s="93"/>
+      <c r="R38" s="94">
         <v>2190</v>
       </c>
-      <c r="S38" s="104"/>
-      <c r="T38" s="105"/>
+      <c r="S38" s="95"/>
+      <c r="T38" s="96"/>
     </row>
     <row r="39" spans="2:27" x14ac:dyDescent="0.2">
       <c r="B39" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="C39" s="92">
+      <c r="C39" s="93">
         <v>4</v>
       </c>
-      <c r="D39" s="92"/>
-      <c r="E39" s="92"/>
-      <c r="F39" s="92"/>
-      <c r="G39" s="92"/>
-      <c r="H39" s="92">
+      <c r="D39" s="93"/>
+      <c r="E39" s="93"/>
+      <c r="F39" s="93"/>
+      <c r="G39" s="93"/>
+      <c r="H39" s="93">
         <v>2</v>
       </c>
-      <c r="I39" s="92"/>
-      <c r="J39" s="92"/>
-      <c r="K39" s="92"/>
-      <c r="L39" s="92"/>
-      <c r="M39" s="92">
+      <c r="I39" s="93"/>
+      <c r="J39" s="93"/>
+      <c r="K39" s="93"/>
+      <c r="L39" s="93"/>
+      <c r="M39" s="93">
         <v>2</v>
       </c>
-      <c r="N39" s="92"/>
-      <c r="O39" s="92"/>
-      <c r="P39" s="92"/>
-      <c r="Q39" s="92"/>
-      <c r="R39" s="103">
+      <c r="N39" s="93"/>
+      <c r="O39" s="93"/>
+      <c r="P39" s="93"/>
+      <c r="Q39" s="93"/>
+      <c r="R39" s="94">
         <v>8</v>
       </c>
-      <c r="S39" s="104"/>
-      <c r="T39" s="105"/>
+      <c r="S39" s="95"/>
+      <c r="T39" s="96"/>
     </row>
     <row r="44" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="R44" s="93" t="s">
+      <c r="R44" s="97" t="s">
         <v>79</v>
       </c>
-      <c r="S44" s="93"/>
-      <c r="T44" s="93"/>
-      <c r="U44" s="93"/>
-      <c r="V44" s="93"/>
-      <c r="W44" s="93"/>
-      <c r="X44" s="93"/>
-      <c r="Y44" s="93"/>
-      <c r="Z44" s="93"/>
-      <c r="AA44" s="93"/>
+      <c r="S44" s="97"/>
+      <c r="T44" s="97"/>
+      <c r="U44" s="97"/>
+      <c r="V44" s="97"/>
+      <c r="W44" s="97"/>
+      <c r="X44" s="97"/>
+      <c r="Y44" s="97"/>
+      <c r="Z44" s="97"/>
+      <c r="AA44" s="97"/>
     </row>
     <row r="45" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="R45" s="98" t="s">
+      <c r="R45" s="103" t="s">
         <v>3</v>
       </c>
-      <c r="S45" s="98"/>
-      <c r="T45" s="98"/>
-      <c r="U45" s="98"/>
-      <c r="V45" s="98"/>
-      <c r="W45" s="99" t="s">
+      <c r="S45" s="103"/>
+      <c r="T45" s="103"/>
+      <c r="U45" s="103"/>
+      <c r="V45" s="103"/>
+      <c r="W45" s="104" t="s">
         <v>4</v>
       </c>
-      <c r="X45" s="99"/>
-      <c r="Y45" s="99"/>
-      <c r="Z45" s="99"/>
-      <c r="AA45" s="99"/>
+      <c r="X45" s="104"/>
+      <c r="Y45" s="104"/>
+      <c r="Z45" s="104"/>
+      <c r="AA45" s="104"/>
     </row>
     <row r="46" spans="2:27" x14ac:dyDescent="0.2">
       <c r="Q46" t="s">
@@ -5094,102 +5094,102 @@
       <c r="Y53" s="21"/>
       <c r="Z53" s="21"/>
       <c r="AA53" s="21"/>
-      <c r="AB53" s="92">
+      <c r="AB53" s="93">
         <v>39</v>
       </c>
-      <c r="AC53" s="92"/>
-      <c r="AD53" s="92"/>
+      <c r="AC53" s="93"/>
+      <c r="AD53" s="93"/>
     </row>
     <row r="54" spans="17:32" x14ac:dyDescent="0.2">
       <c r="Q54" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="R54" s="103">
+      <c r="R54" s="94">
         <v>16</v>
       </c>
-      <c r="S54" s="104"/>
-      <c r="T54" s="104"/>
-      <c r="U54" s="104"/>
-      <c r="V54" s="105"/>
-      <c r="W54" s="92">
+      <c r="S54" s="95"/>
+      <c r="T54" s="95"/>
+      <c r="U54" s="95"/>
+      <c r="V54" s="96"/>
+      <c r="W54" s="93">
         <v>23</v>
       </c>
-      <c r="X54" s="92"/>
-      <c r="Y54" s="92"/>
-      <c r="Z54" s="92"/>
-      <c r="AA54" s="92"/>
-      <c r="AB54" s="103">
+      <c r="X54" s="93"/>
+      <c r="Y54" s="93"/>
+      <c r="Z54" s="93"/>
+      <c r="AA54" s="93"/>
+      <c r="AB54" s="94">
         <v>1170</v>
       </c>
-      <c r="AC54" s="104"/>
-      <c r="AD54" s="105"/>
+      <c r="AC54" s="95"/>
+      <c r="AD54" s="96"/>
     </row>
     <row r="55" spans="17:32" x14ac:dyDescent="0.2">
       <c r="Q55" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="R55" s="103">
+      <c r="R55" s="94">
         <v>480</v>
       </c>
-      <c r="S55" s="104"/>
-      <c r="T55" s="104"/>
-      <c r="U55" s="104"/>
-      <c r="V55" s="105"/>
-      <c r="W55" s="92">
+      <c r="S55" s="95"/>
+      <c r="T55" s="95"/>
+      <c r="U55" s="95"/>
+      <c r="V55" s="96"/>
+      <c r="W55" s="93">
         <v>690</v>
       </c>
-      <c r="X55" s="92"/>
-      <c r="Y55" s="92"/>
-      <c r="Z55" s="92"/>
-      <c r="AA55" s="92"/>
-      <c r="AB55" s="103">
+      <c r="X55" s="93"/>
+      <c r="Y55" s="93"/>
+      <c r="Z55" s="93"/>
+      <c r="AA55" s="93"/>
+      <c r="AB55" s="94">
         <v>4</v>
       </c>
-      <c r="AC55" s="104"/>
-      <c r="AD55" s="105"/>
+      <c r="AC55" s="95"/>
+      <c r="AD55" s="96"/>
     </row>
     <row r="56" spans="17:32" x14ac:dyDescent="0.2">
       <c r="Q56" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="R56" s="103">
+      <c r="R56" s="94">
         <v>2</v>
       </c>
-      <c r="S56" s="104"/>
-      <c r="T56" s="104"/>
-      <c r="U56" s="104"/>
-      <c r="V56" s="105"/>
-      <c r="W56" s="92">
+      <c r="S56" s="95"/>
+      <c r="T56" s="95"/>
+      <c r="U56" s="95"/>
+      <c r="V56" s="96"/>
+      <c r="W56" s="93">
         <v>2</v>
       </c>
-      <c r="X56" s="92"/>
-      <c r="Y56" s="92"/>
-      <c r="Z56" s="92"/>
-      <c r="AA56" s="92"/>
-      <c r="AB56" s="103" t="e">
+      <c r="X56" s="93"/>
+      <c r="Y56" s="93"/>
+      <c r="Z56" s="93"/>
+      <c r="AA56" s="93"/>
+      <c r="AB56" s="94" t="e">
         <f>SUM(W56,R56,M56,#REF!,#REF!,#REF!)</f>
         <v>#REF!</v>
       </c>
-      <c r="AC56" s="104"/>
-      <c r="AD56" s="105"/>
+      <c r="AC56" s="95"/>
+      <c r="AD56" s="96"/>
     </row>
     <row r="61" spans="17:32" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="AB61" s="94" t="s">
+      <c r="AB61" s="108" t="s">
         <v>80</v>
       </c>
-      <c r="AC61" s="94"/>
-      <c r="AD61" s="94"/>
-      <c r="AE61" s="94"/>
-      <c r="AF61" s="94"/>
+      <c r="AC61" s="108"/>
+      <c r="AD61" s="108"/>
+      <c r="AE61" s="108"/>
+      <c r="AF61" s="108"/>
     </row>
     <row r="62" spans="17:32" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="AB62" s="100" t="s">
+      <c r="AB62" s="112" t="s">
         <v>5</v>
       </c>
-      <c r="AC62" s="101"/>
-      <c r="AD62" s="101"/>
-      <c r="AE62" s="101"/>
-      <c r="AF62" s="102"/>
+      <c r="AC62" s="113"/>
+      <c r="AD62" s="113"/>
+      <c r="AE62" s="113"/>
+      <c r="AF62" s="114"/>
     </row>
     <row r="63" spans="17:32" ht="16" thickTop="1" x14ac:dyDescent="0.2">
       <c r="AA63" t="s">
@@ -5302,62 +5302,62 @@
       <c r="AD70" s="21"/>
       <c r="AE70" s="21"/>
       <c r="AF70" s="21"/>
-      <c r="AG70" s="92" t="s">
+      <c r="AG70" s="93" t="s">
         <v>88</v>
       </c>
-      <c r="AH70" s="92"/>
-      <c r="AI70" s="92"/>
+      <c r="AH70" s="93"/>
+      <c r="AI70" s="93"/>
     </row>
     <row r="71" spans="3:35" x14ac:dyDescent="0.2">
       <c r="AA71" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="AB71" s="92">
+      <c r="AB71" s="93">
         <v>9</v>
       </c>
-      <c r="AC71" s="92"/>
-      <c r="AD71" s="92"/>
-      <c r="AE71" s="92"/>
-      <c r="AF71" s="92"/>
-      <c r="AG71" s="103">
+      <c r="AC71" s="93"/>
+      <c r="AD71" s="93"/>
+      <c r="AE71" s="93"/>
+      <c r="AF71" s="93"/>
+      <c r="AG71" s="94">
         <v>9</v>
       </c>
-      <c r="AH71" s="104"/>
-      <c r="AI71" s="105"/>
+      <c r="AH71" s="95"/>
+      <c r="AI71" s="96"/>
     </row>
     <row r="72" spans="3:35" x14ac:dyDescent="0.2">
       <c r="AA72" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="AB72" s="92">
+      <c r="AB72" s="93">
         <v>270</v>
       </c>
-      <c r="AC72" s="92"/>
-      <c r="AD72" s="92"/>
-      <c r="AE72" s="92"/>
-      <c r="AF72" s="92"/>
-      <c r="AG72" s="103">
+      <c r="AC72" s="93"/>
+      <c r="AD72" s="93"/>
+      <c r="AE72" s="93"/>
+      <c r="AF72" s="93"/>
+      <c r="AG72" s="94">
         <v>270</v>
       </c>
-      <c r="AH72" s="104"/>
-      <c r="AI72" s="105"/>
+      <c r="AH72" s="95"/>
+      <c r="AI72" s="96"/>
     </row>
     <row r="73" spans="3:35" x14ac:dyDescent="0.2">
       <c r="AA73" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="AB73" s="92">
+      <c r="AB73" s="93">
         <v>2</v>
       </c>
-      <c r="AC73" s="92"/>
-      <c r="AD73" s="92"/>
-      <c r="AE73" s="92"/>
-      <c r="AF73" s="92"/>
-      <c r="AG73" s="103">
+      <c r="AC73" s="93"/>
+      <c r="AD73" s="93"/>
+      <c r="AE73" s="93"/>
+      <c r="AF73" s="93"/>
+      <c r="AG73" s="94">
         <v>2</v>
       </c>
-      <c r="AH73" s="104"/>
-      <c r="AI73" s="105"/>
+      <c r="AH73" s="95"/>
+      <c r="AI73" s="96"/>
     </row>
     <row r="75" spans="3:35" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="76" spans="3:35" x14ac:dyDescent="0.2">
@@ -5375,24 +5375,24 @@
       <c r="S77" s="89"/>
     </row>
     <row r="78" spans="3:35" x14ac:dyDescent="0.2">
-      <c r="C78" s="106" t="s">
+      <c r="C78" s="105" t="s">
         <v>64</v>
       </c>
-      <c r="D78" s="107"/>
-      <c r="E78" s="107"/>
-      <c r="F78" s="107"/>
-      <c r="G78" s="107"/>
-      <c r="H78" s="107"/>
-      <c r="I78" s="108"/>
-      <c r="J78" s="106" t="s">
+      <c r="D78" s="106"/>
+      <c r="E78" s="106"/>
+      <c r="F78" s="106"/>
+      <c r="G78" s="106"/>
+      <c r="H78" s="106"/>
+      <c r="I78" s="107"/>
+      <c r="J78" s="105" t="s">
         <v>73</v>
       </c>
-      <c r="K78" s="107"/>
-      <c r="L78" s="107"/>
-      <c r="M78" s="107"/>
-      <c r="N78" s="107"/>
-      <c r="O78" s="107"/>
-      <c r="P78" s="108"/>
+      <c r="K78" s="106"/>
+      <c r="L78" s="106"/>
+      <c r="M78" s="106"/>
+      <c r="N78" s="106"/>
+      <c r="O78" s="106"/>
+      <c r="P78" s="107"/>
       <c r="R78" s="9">
         <v>1</v>
       </c>
@@ -5669,14 +5669,14 @@
       <c r="S84" s="17"/>
     </row>
     <row r="90" spans="3:19" x14ac:dyDescent="0.2">
-      <c r="C90" s="92" t="s">
+      <c r="C90" s="93" t="s">
         <v>84</v>
       </c>
-      <c r="D90" s="92"/>
-      <c r="E90" s="92"/>
-      <c r="G90" s="113"/>
-      <c r="H90" s="113"/>
-      <c r="I90" s="113"/>
+      <c r="D90" s="93"/>
+      <c r="E90" s="93"/>
+      <c r="G90" s="98"/>
+      <c r="H90" s="98"/>
+      <c r="I90" s="98"/>
     </row>
     <row r="91" spans="3:19" x14ac:dyDescent="0.2">
       <c r="C91" s="5" t="s">
@@ -5805,14 +5805,14 @@
       <c r="I99" s="91"/>
     </row>
     <row r="102" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C102" s="92" t="s">
+      <c r="C102" s="93" t="s">
         <v>86</v>
       </c>
-      <c r="D102" s="92"/>
-      <c r="E102" s="92"/>
-      <c r="F102" s="92"/>
-      <c r="G102" s="92"/>
-      <c r="H102" s="92"/>
+      <c r="D102" s="93"/>
+      <c r="E102" s="93"/>
+      <c r="F102" s="93"/>
+      <c r="G102" s="93"/>
+      <c r="H102" s="93"/>
     </row>
     <row r="103" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C103" s="5" t="s">
@@ -5839,13 +5839,13 @@
         <v>1</v>
       </c>
       <c r="D104" s="83">
-        <v>44890</v>
+        <v>44891</v>
       </c>
       <c r="E104" s="83">
-        <v>44890</v>
+        <v>44891</v>
       </c>
       <c r="F104" s="83">
-        <v>44890</v>
+        <v>44891</v>
       </c>
       <c r="G104" s="83">
         <v>44893</v>
@@ -5913,7 +5913,7 @@
       <c r="H107" s="83">
         <v>44907</v>
       </c>
-      <c r="I107" s="114"/>
+      <c r="I107" s="92"/>
       <c r="J107" s="90"/>
     </row>
     <row r="108" spans="3:10" x14ac:dyDescent="0.2">
@@ -5958,6 +5958,51 @@
     </row>
   </sheetData>
   <mergeCells count="61">
+    <mergeCell ref="AB72:AF72"/>
+    <mergeCell ref="AB73:AF73"/>
+    <mergeCell ref="R44:AA44"/>
+    <mergeCell ref="AB61:AF61"/>
+    <mergeCell ref="C28:G28"/>
+    <mergeCell ref="H28:L28"/>
+    <mergeCell ref="M28:Q28"/>
+    <mergeCell ref="R45:V45"/>
+    <mergeCell ref="W45:AA45"/>
+    <mergeCell ref="AB62:AF62"/>
+    <mergeCell ref="R56:V56"/>
+    <mergeCell ref="W54:AA54"/>
+    <mergeCell ref="W55:AA55"/>
+    <mergeCell ref="W56:AA56"/>
+    <mergeCell ref="AB71:AF71"/>
+    <mergeCell ref="C102:H102"/>
+    <mergeCell ref="C78:I78"/>
+    <mergeCell ref="AG22:AI22"/>
+    <mergeCell ref="AG23:AI23"/>
+    <mergeCell ref="AG24:AI24"/>
+    <mergeCell ref="J78:P78"/>
+    <mergeCell ref="C27:Q27"/>
+    <mergeCell ref="C37:G37"/>
+    <mergeCell ref="C38:G38"/>
+    <mergeCell ref="C39:G39"/>
+    <mergeCell ref="H37:L37"/>
+    <mergeCell ref="H38:L38"/>
+    <mergeCell ref="H39:L39"/>
+    <mergeCell ref="M37:Q37"/>
+    <mergeCell ref="M38:Q38"/>
+    <mergeCell ref="M39:Q39"/>
+    <mergeCell ref="AB14:AF14"/>
+    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="H14:L14"/>
+    <mergeCell ref="M14:Q14"/>
+    <mergeCell ref="R14:V14"/>
+    <mergeCell ref="W14:AA14"/>
+    <mergeCell ref="C90:E90"/>
+    <mergeCell ref="R36:T36"/>
+    <mergeCell ref="R37:T37"/>
+    <mergeCell ref="R38:T38"/>
+    <mergeCell ref="R39:T39"/>
+    <mergeCell ref="R54:V54"/>
+    <mergeCell ref="R55:V55"/>
+    <mergeCell ref="G90:I90"/>
     <mergeCell ref="AG70:AI70"/>
     <mergeCell ref="AG71:AI71"/>
     <mergeCell ref="AG72:AI72"/>
@@ -5974,51 +6019,6 @@
     <mergeCell ref="W23:AA23"/>
     <mergeCell ref="AB25:AF25"/>
     <mergeCell ref="W25:AA25"/>
-    <mergeCell ref="C90:E90"/>
-    <mergeCell ref="R36:T36"/>
-    <mergeCell ref="R37:T37"/>
-    <mergeCell ref="R38:T38"/>
-    <mergeCell ref="R39:T39"/>
-    <mergeCell ref="R54:V54"/>
-    <mergeCell ref="R55:V55"/>
-    <mergeCell ref="G90:I90"/>
-    <mergeCell ref="AB14:AF14"/>
-    <mergeCell ref="C14:G14"/>
-    <mergeCell ref="H14:L14"/>
-    <mergeCell ref="M14:Q14"/>
-    <mergeCell ref="R14:V14"/>
-    <mergeCell ref="W14:AA14"/>
-    <mergeCell ref="C102:H102"/>
-    <mergeCell ref="C78:I78"/>
-    <mergeCell ref="AG22:AI22"/>
-    <mergeCell ref="AG23:AI23"/>
-    <mergeCell ref="AG24:AI24"/>
-    <mergeCell ref="J78:P78"/>
-    <mergeCell ref="C27:Q27"/>
-    <mergeCell ref="C37:G37"/>
-    <mergeCell ref="C38:G38"/>
-    <mergeCell ref="C39:G39"/>
-    <mergeCell ref="H37:L37"/>
-    <mergeCell ref="H38:L38"/>
-    <mergeCell ref="H39:L39"/>
-    <mergeCell ref="M37:Q37"/>
-    <mergeCell ref="M38:Q38"/>
-    <mergeCell ref="M39:Q39"/>
-    <mergeCell ref="AB72:AF72"/>
-    <mergeCell ref="AB73:AF73"/>
-    <mergeCell ref="R44:AA44"/>
-    <mergeCell ref="AB61:AF61"/>
-    <mergeCell ref="C28:G28"/>
-    <mergeCell ref="H28:L28"/>
-    <mergeCell ref="M28:Q28"/>
-    <mergeCell ref="R45:V45"/>
-    <mergeCell ref="W45:AA45"/>
-    <mergeCell ref="AB62:AF62"/>
-    <mergeCell ref="R56:V56"/>
-    <mergeCell ref="W54:AA54"/>
-    <mergeCell ref="W55:AA55"/>
-    <mergeCell ref="W56:AA56"/>
-    <mergeCell ref="AB71:AF71"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>